<commit_message>
Revert "started to add fake news functionality"
This reverts commit 3612389cc8ffa280bbfcfefeb4a495f60c28f44f.
</commit_message>
<xml_diff>
--- a/HelplinePlatform-Issues-PendingAndNew-20191101.xlsx
+++ b/HelplinePlatform-Issues-PendingAndNew-20191101.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oneoc\Desktop\ICTOU project\CyberSafeReportingToolIII\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iacovosi\cybersafe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F1FDCB-655F-426D-BD79-C2E052617126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -919,7 +918,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1192,8 +1191,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A3:F41" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A3:F41" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:F41" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A3:F41">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1202,12 +1201,12 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="#" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Description" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Σελίδα" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Comments" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Status" dataDxfId="0"/>
+    <tableColumn id="4" name="#" dataDxfId="5"/>
+    <tableColumn id="1" name="Description" dataDxfId="4"/>
+    <tableColumn id="2" name="Σελίδα" dataDxfId="3"/>
+    <tableColumn id="3" name="Type" dataDxfId="2"/>
+    <tableColumn id="6" name="Comments" dataDxfId="1"/>
+    <tableColumn id="7" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1475,26 +1474,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="92" style="1" customWidth="1"/>
-    <col min="3" max="3" width="0.7265625" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.7265625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="66.81640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.81640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="1"/>
+    <col min="3" max="3" width="0.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="66.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1502,7 +1501,7 @@
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
     </row>
-    <row r="3" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
@@ -1525,7 +1524,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
         <v>5</v>
@@ -1535,7 +1534,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -1556,7 +1555,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -1577,7 +1576,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -1595,7 +1594,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -1618,7 +1617,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="174" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -1636,7 +1635,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -1655,7 +1654,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>3</v>
@@ -1665,7 +1664,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>7</v>
       </c>
@@ -1684,7 +1683,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>8</v>
       </c>
@@ -1703,7 +1702,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>9</v>
       </c>
@@ -1723,7 +1722,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>10</v>
       </c>
@@ -1742,7 +1741,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>11</v>
       </c>
@@ -1760,7 +1759,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>12</v>
       </c>
@@ -1777,7 +1776,7 @@
       </c>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:8" ht="116" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>13</v>
       </c>
@@ -1799,7 +1798,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>14</v>
       </c>
@@ -1818,7 +1817,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>15</v>
       </c>
@@ -1837,7 +1836,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>16</v>
       </c>
@@ -1856,7 +1855,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>17</v>
       </c>
@@ -1872,7 +1871,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
         <v>67</v>
@@ -1884,7 +1883,7 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
         <v>70</v>
@@ -1899,7 +1898,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6" t="s">
         <v>4</v>
@@ -1910,7 +1909,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>18</v>
       </c>
@@ -1929,7 +1928,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>19</v>
       </c>
@@ -1948,7 +1947,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>20</v>
       </c>
@@ -1965,7 +1964,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>21</v>
       </c>
@@ -1984,7 +1983,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>22</v>
       </c>
@@ -2003,7 +2002,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>23</v>
       </c>
@@ -2022,7 +2021,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>24</v>
       </c>
@@ -2039,7 +2038,7 @@
       </c>
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>25</v>
       </c>
@@ -2058,7 +2057,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>26</v>
       </c>
@@ -2072,7 +2071,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="4" t="s">
         <v>69</v>
@@ -2087,7 +2086,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6" t="s">
         <v>29</v>
@@ -2097,7 +2096,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>27</v>
       </c>
@@ -2114,7 +2113,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6" t="s">
         <v>30</v>
@@ -2124,7 +2123,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>28</v>
       </c>
@@ -2138,7 +2137,7 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6" t="s">
         <v>31</v>
@@ -2148,7 +2147,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>29</v>
       </c>
@@ -2162,7 +2161,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2182,19 +2181,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
@@ -2208,7 +2207,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2219,21 +2218,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C22A0549F0780D44A515DAC593D990C1" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="77a25ec2ce495eca88f50c42d265dff3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="23c82419-2300-4e96-abf4-1c91944b2283" xmlns:ns3="3d1315c4-4db4-43e5-ade1-45c47b3ecb5d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d80f2f4478354c409078d8e2e9daa312" ns2:_="" ns3:_="">
     <xsd:import namespace="23c82419-2300-4e96-abf4-1c91944b2283"/>
@@ -2436,32 +2420,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5DD2DC9-1E3C-49EE-BC04-8A68ED3BD415}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3d1315c4-4db4-43e5-ade1-45c47b3ecb5d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="23c82419-2300-4e96-abf4-1c91944b2283"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1618630E-44B8-49E0-BBF2-8C63396302BE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFE7056-B389-4B85-A995-621B9D656540}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2478,4 +2452,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1618630E-44B8-49E0-BBF2-8C63396302BE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5DD2DC9-1E3C-49EE-BC04-8A68ED3BD415}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="3d1315c4-4db4-43e5-ade1-45c47b3ecb5d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="23c82419-2300-4e96-abf4-1c91944b2283"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>